<commit_message>
working NNetwork on single point, style revisions, test
</commit_message>
<xml_diff>
--- a/model.xlsx
+++ b/model.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="13">
   <si>
     <t>Vii</t>
   </si>
@@ -544,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M44" sqref="M44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,102 +936,713 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="7">
+        <v>10</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="D16" s="14">
         <f>D2+D3*0.01</f>
         <v>1.2</v>
       </c>
+      <c r="E16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="7">
+        <f>B16*D16</f>
+        <v>12</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="H16" s="14">
-        <v>1</v>
-      </c>
-      <c r="L16" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D17" s="5"/>
-      <c r="H17" s="5">
         <f>H2+H3*0.01</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="L17" s="5">
+      <c r="I16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="7">
+        <f>(F16*H16+F18*H18)</f>
+        <v>14.21</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" s="14">
         <f>L2+L3*0.01</f>
         <v>1.1100000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N16" s="8">
+        <f>J16*L16+J21*L21+J26*L26</f>
+        <v>32.556200000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="5">
+        <f>(F17+F22)*B16</f>
+        <v>24.420000000000005</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1">
+        <f>H16*J17</f>
+        <v>1.2210000000000003</v>
+      </c>
+      <c r="G17" s="12"/>
+      <c r="H17" s="5">
+        <f>J17*F16</f>
+        <v>13.32</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J17" s="1">
+        <f>L16*N17</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="K17" s="12"/>
+      <c r="L17" s="5">
+        <f>J16*N17</f>
+        <v>14.21</v>
+      </c>
+      <c r="M17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
       <c r="D18" s="5"/>
+      <c r="E18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="H18" s="14">
-        <v>1</v>
-      </c>
-      <c r="L18" s="5"/>
-    </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D19" s="5"/>
-      <c r="H19" s="5">
         <f>H4+H5*0.01</f>
         <v>1.01</v>
       </c>
+      <c r="I18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="7"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N18" s="8"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="2">
+        <f>H18*J17</f>
+        <v>1.1211000000000002</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="5">
+        <f>F18*J17</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="I19" s="9"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="10"/>
       <c r="L19" s="5"/>
-    </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19" s="10"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
       <c r="H20" s="4"/>
       <c r="L20" s="4"/>
-    </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="5"/>
+      <c r="E21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="7">
+        <f>B16*D16</f>
+        <v>12</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="H21" s="14">
-        <v>1</v>
-      </c>
-      <c r="L21" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D22" s="5"/>
-      <c r="H22" s="5">
         <f>H7+H8*0.01</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="L22" s="5">
+      <c r="I21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="7">
+        <f>(F21*H21+F23*H23)</f>
+        <v>14.21</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21" s="14">
         <f>L7+L8*0.01</f>
         <v>1.1100000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N21" s="8"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="1">
+        <f>H21*J22</f>
+        <v>1.2210000000000003</v>
+      </c>
+      <c r="G22" s="12"/>
+      <c r="H22" s="5">
+        <f>F21*J22</f>
+        <v>13.32</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J22" s="1">
+        <f>L21*N17</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="K22" s="12"/>
+      <c r="L22" s="5">
+        <f>J21*N17</f>
+        <v>14.21</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N22" s="12"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7">
+        <v>1</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="H23" s="14">
-        <v>1</v>
-      </c>
-      <c r="L23" s="5"/>
-    </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D24" s="5"/>
-      <c r="H24" s="5">
         <f>H9+H10*0.01</f>
         <v>1.01</v>
       </c>
+      <c r="I23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="7"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N23" s="8"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="2">
+        <f>H23*J22</f>
+        <v>1.1211000000000002</v>
+      </c>
+      <c r="G24" s="10"/>
+      <c r="H24" s="5">
+        <f>F23*J22</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="10"/>
       <c r="L24" s="5"/>
-    </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N24" s="10"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D25" s="4"/>
       <c r="H25" s="4"/>
       <c r="L25" s="4"/>
-    </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="8"/>
       <c r="D26" s="5"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="8"/>
       <c r="H26" s="5"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="7">
+        <v>1</v>
+      </c>
+      <c r="K26" s="8" t="s">
+        <v>9</v>
+      </c>
       <c r="L26" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="L27" s="13">
         <f>L12+L13*0.01</f>
         <v>1.01</v>
       </c>
+      <c r="M26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N26" s="8"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="2">
+        <f>L26*N17</f>
+        <v>1.01</v>
+      </c>
+      <c r="K27" s="10"/>
+      <c r="L27" s="13">
+        <f>J26*N17</f>
+        <v>1</v>
+      </c>
+      <c r="M27" s="9"/>
+      <c r="N27" s="10"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="7">
+        <v>10</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="14">
+        <f>D16+D17*0.01</f>
+        <v>1.4441999999999999</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="7">
+        <f>B30*D30</f>
+        <v>14.442</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="14">
+        <f>H16+H17*0.01</f>
+        <v>1.2332000000000001</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" s="7">
+        <f>(F30*H30+F32*H32)</f>
+        <v>18.830974400000002</v>
+      </c>
+      <c r="K30" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L30" s="14">
+        <f>L16+L17*0.01</f>
+        <v>1.2521</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N30" s="8">
+        <f>J30*L30+J35*L35+J40*L40</f>
+        <v>48.17652609248001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="5">
+        <f>(F31+F36)*B30</f>
+        <v>30.881794400000004</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" s="1">
+        <f>H30*J31</f>
+        <v>1.5440897200000001</v>
+      </c>
+      <c r="G31" s="12"/>
+      <c r="H31" s="5">
+        <f>J31*F30</f>
+        <v>18.082828200000002</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J31" s="1">
+        <f>L30*N31</f>
+        <v>1.2521</v>
+      </c>
+      <c r="K31" s="12"/>
+      <c r="L31" s="5">
+        <f>J30*N31</f>
+        <v>18.830974400000002</v>
+      </c>
+      <c r="M31" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N31" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="7">
+        <v>1</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="14">
+        <f>H18+H19*0.01</f>
+        <v>1.0211000000000001</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" s="7"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N32" s="8"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="2">
+        <f>H32*J31</f>
+        <v>1.2785193100000001</v>
+      </c>
+      <c r="G33" s="10"/>
+      <c r="H33" s="5">
+        <f>F32*J31</f>
+        <v>1.2521</v>
+      </c>
+      <c r="I33" s="9"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N33" s="10"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D34" s="4"/>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="7">
+        <f>B30*D30</f>
+        <v>14.442</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35" s="14">
+        <f>H21+H22*0.01</f>
+        <v>1.2332000000000001</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J35" s="7">
+        <f>(F35*H35+F37*H37)</f>
+        <v>18.830974400000002</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L35" s="14">
+        <f>L21+L22*0.01</f>
+        <v>1.2521</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N35" s="8"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="1">
+        <f>H35*J36</f>
+        <v>1.5440897200000001</v>
+      </c>
+      <c r="G36" s="12"/>
+      <c r="H36" s="5">
+        <f>F35*J36</f>
+        <v>18.082828200000002</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="1">
+        <f>L35*N31</f>
+        <v>1.2521</v>
+      </c>
+      <c r="K36" s="12"/>
+      <c r="L36" s="5">
+        <f>J35*N31</f>
+        <v>18.830974400000002</v>
+      </c>
+      <c r="M36" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N36" s="12"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="7">
+        <v>1</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="14">
+        <f>H23+H24*0.01</f>
+        <v>1.0211000000000001</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J37" s="7"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N37" s="8"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="2">
+        <f>H37*J36</f>
+        <v>1.2785193100000001</v>
+      </c>
+      <c r="G38" s="10"/>
+      <c r="H38" s="5">
+        <f>F37*J36</f>
+        <v>1.2521</v>
+      </c>
+      <c r="I38" s="9"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N38" s="10"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="7">
+        <v>1</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L40" s="14">
+        <f>L26+L27*0.01</f>
+        <v>1.02</v>
+      </c>
+      <c r="M40" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N40" s="8"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="2">
+        <f>L40*N31</f>
+        <v>1.02</v>
+      </c>
+      <c r="K41" s="10"/>
+      <c r="L41" s="13">
+        <f>J40*N31</f>
+        <v>1</v>
+      </c>
+      <c r="M41" s="9"/>
+      <c r="N41" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added tests, few comments and behavior
</commit_message>
<xml_diff>
--- a/model.xlsx
+++ b/model.xlsx
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,46 +588,46 @@
         <v>7</v>
       </c>
       <c r="B2" s="7">
-        <v>10</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="5">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="7">
         <f>B2*D2</f>
-        <v>10</v>
+        <v>5.5</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="5">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="7">
         <f>(F2*H2+F4*H4)</f>
-        <v>11</v>
+        <v>16.25</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L2" s="5">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N2" s="8">
         <f>J2*L2+J7*L7+J12*L12</f>
-        <v>23</v>
+        <v>83.75</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -638,31 +638,31 @@
       <c r="C3" s="12"/>
       <c r="D3" s="5">
         <f>(F3+F8)*B2</f>
-        <v>20</v>
+        <v>27.500000000000004</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="1">
         <f>H2*J3</f>
-        <v>1</v>
+        <v>6.25</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="5">
         <f>J3*F2</f>
-        <v>10</v>
+        <v>13.75</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J3" s="1">
         <f>L2*N3</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="K3" s="12"/>
       <c r="L3" s="5">
         <f>J2*N3</f>
-        <v>11</v>
+        <v>16.25</v>
       </c>
       <c r="M3" s="11" t="s">
         <v>11</v>
@@ -688,7 +688,7 @@
         <v>9</v>
       </c>
       <c r="H4" s="5">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>11</v>
@@ -713,12 +713,12 @@
       </c>
       <c r="F5" s="2">
         <f>H4*J3</f>
-        <v>1</v>
+        <v>6.25</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="5">
         <f>F4*J3</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="2"/>
@@ -752,26 +752,26 @@
       </c>
       <c r="F7" s="7">
         <f>B2*D2</f>
-        <v>10</v>
+        <v>5.5</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="5">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J7" s="7">
         <f>(F7*H7+F9*H9)</f>
-        <v>11</v>
+        <v>16.25</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L7" s="5">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>11</v>
@@ -788,24 +788,24 @@
       <c r="E8" s="11"/>
       <c r="F8" s="1">
         <f>H7*J8</f>
-        <v>1</v>
+        <v>6.25</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="5">
         <f>F7*J8</f>
-        <v>10</v>
+        <v>13.75</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J8" s="1">
         <f>L7*N3</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="K8" s="12"/>
       <c r="L8" s="5">
         <f>J7*N3</f>
-        <v>11</v>
+        <v>16.25</v>
       </c>
       <c r="M8" s="11" t="s">
         <v>11</v>
@@ -827,7 +827,7 @@
         <v>9</v>
       </c>
       <c r="H9" s="5">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>11</v>
@@ -850,12 +850,12 @@
       <c r="E10" s="9"/>
       <c r="F10" s="2">
         <f>H9*J8</f>
-        <v>1</v>
+        <v>6.25</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="5">
         <f>F9*J8</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="2"/>
@@ -893,7 +893,7 @@
         <v>9</v>
       </c>
       <c r="L12" s="5">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="M12" s="6" t="s">
         <v>11</v>
@@ -914,7 +914,7 @@
       <c r="I13" s="9"/>
       <c r="J13" s="2">
         <f>L12*N3</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="13">
@@ -947,42 +947,42 @@
       </c>
       <c r="D16" s="14">
         <f>D2+D3*0.01</f>
-        <v>1.2</v>
+        <v>2.7749999999999999</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="7">
         <f>B16*D16</f>
-        <v>12</v>
+        <v>27.75</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="14">
         <f>H2+H3*0.01</f>
-        <v>1.1000000000000001</v>
+        <v>2.6375000000000002</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J16" s="7">
         <f>(F16*H16+F18*H18)</f>
-        <v>14.21</v>
+        <v>75.715625000000017</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L16" s="14">
         <f>L2+L3*0.01</f>
-        <v>1.1100000000000001</v>
+        <v>2.6625000000000001</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N16" s="8">
         <f>J16*L16+J21*L21+J26*L26</f>
-        <v>32.556200000000004</v>
+        <v>405.69570312500008</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -993,31 +993,31 @@
       <c r="C17" s="12"/>
       <c r="D17" s="5">
         <f>(F17+F22)*B16</f>
-        <v>24.420000000000005</v>
+        <v>140.44687500000003</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="1">
         <f>H16*J17</f>
-        <v>1.2210000000000003</v>
+        <v>7.022343750000001</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="5">
         <f>J17*F16</f>
-        <v>13.32</v>
+        <v>73.884375000000006</v>
       </c>
       <c r="I17" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J17" s="1">
         <f>L16*N17</f>
-        <v>1.1100000000000001</v>
+        <v>2.6625000000000001</v>
       </c>
       <c r="K17" s="12"/>
       <c r="L17" s="5">
         <f>J16*N17</f>
-        <v>14.21</v>
+        <v>75.715625000000017</v>
       </c>
       <c r="M17" s="11" t="s">
         <v>11</v>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="H18" s="14">
         <f>H4+H5*0.01</f>
-        <v>1.01</v>
+        <v>2.5249999999999999</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>11</v>
@@ -1069,12 +1069,12 @@
       </c>
       <c r="F19" s="2">
         <f>H18*J17</f>
-        <v>1.1211000000000002</v>
+        <v>6.7228124999999999</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="5">
         <f>F18*J17</f>
-        <v>1.1100000000000001</v>
+        <v>2.6625000000000001</v>
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="2"/>
@@ -1108,28 +1108,28 @@
       </c>
       <c r="F21" s="7">
         <f>B16*D16</f>
-        <v>12</v>
+        <v>27.75</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H21" s="14">
         <f>H7+H8*0.01</f>
-        <v>1.1000000000000001</v>
+        <v>2.6375000000000002</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J21" s="7">
         <f>(F21*H21+F23*H23)</f>
-        <v>14.21</v>
+        <v>75.715625000000017</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L21" s="14">
         <f>L7+L8*0.01</f>
-        <v>1.1100000000000001</v>
+        <v>2.6625000000000001</v>
       </c>
       <c r="M21" s="6" t="s">
         <v>11</v>
@@ -1146,24 +1146,24 @@
       <c r="E22" s="11"/>
       <c r="F22" s="1">
         <f>H21*J22</f>
-        <v>1.2210000000000003</v>
+        <v>7.022343750000001</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="5">
         <f>F21*J22</f>
-        <v>13.32</v>
+        <v>73.884375000000006</v>
       </c>
       <c r="I22" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J22" s="1">
         <f>L21*N17</f>
-        <v>1.1100000000000001</v>
+        <v>2.6625000000000001</v>
       </c>
       <c r="K22" s="12"/>
       <c r="L22" s="5">
         <f>J21*N17</f>
-        <v>14.21</v>
+        <v>75.715625000000017</v>
       </c>
       <c r="M22" s="11" t="s">
         <v>11</v>
@@ -1186,7 +1186,7 @@
       </c>
       <c r="H23" s="14">
         <f>H9+H10*0.01</f>
-        <v>1.01</v>
+        <v>2.5249999999999999</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>11</v>
@@ -1209,12 +1209,12 @@
       <c r="E24" s="9"/>
       <c r="F24" s="2">
         <f>H23*J22</f>
-        <v>1.1211000000000002</v>
+        <v>6.7228124999999999</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="5">
         <f>F23*J22</f>
-        <v>1.1100000000000001</v>
+        <v>2.6625000000000001</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="2"/>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="L26" s="14">
         <f>L12+L13*0.01</f>
-        <v>1.01</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="M26" s="6" t="s">
         <v>11</v>
@@ -1274,7 +1274,7 @@
       <c r="I27" s="9"/>
       <c r="J27" s="2">
         <f>L26*N17</f>
-        <v>1.01</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="K27" s="10"/>
       <c r="L27" s="13">
@@ -1307,42 +1307,42 @@
       </c>
       <c r="D30" s="14">
         <f>D16+D17*0.01</f>
-        <v>1.4441999999999999</v>
+        <v>4.1794687499999998</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F30" s="7">
         <f>B30*D30</f>
-        <v>14.442</v>
+        <v>41.794687499999995</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H30" s="14">
         <f>H16+H17*0.01</f>
-        <v>1.2332000000000001</v>
+        <v>3.3763437500000002</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J30" s="7">
         <f>(F30*H30+F32*H32)</f>
-        <v>18.830974400000002</v>
+        <v>143.66485692382813</v>
       </c>
       <c r="K30" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L30" s="14">
         <f>L16+L17*0.01</f>
-        <v>1.2521</v>
+        <v>3.4196562500000001</v>
       </c>
       <c r="M30" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N30" s="8">
         <f>J30*L30+J35*L35+J40*L40</f>
-        <v>48.17652609248001</v>
+        <v>985.08885176984927</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -1353,31 +1353,31 @@
       <c r="C31" s="12"/>
       <c r="D31" s="5">
         <f>(F31+F36)*B30</f>
-        <v>30.881794400000004</v>
+        <v>230.91870013671877</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F31" s="1">
         <f>H30*J31</f>
-        <v>1.5440897200000001</v>
+        <v>11.545935006835938</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="5">
         <f>J31*F30</f>
-        <v>18.082828200000002</v>
+        <v>142.92346432617185</v>
       </c>
       <c r="I31" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J31" s="1">
         <f>L30*N31</f>
-        <v>1.2521</v>
+        <v>3.4196562500000001</v>
       </c>
       <c r="K31" s="12"/>
       <c r="L31" s="5">
         <f>J30*N31</f>
-        <v>18.830974400000002</v>
+        <v>143.66485692382813</v>
       </c>
       <c r="M31" s="11" t="s">
         <v>11</v>
@@ -1404,7 +1404,7 @@
       </c>
       <c r="H32" s="14">
         <f>H18+H19*0.01</f>
-        <v>1.0211000000000001</v>
+        <v>2.551625</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>11</v>
@@ -1429,12 +1429,12 @@
       </c>
       <c r="F33" s="2">
         <f>H32*J31</f>
-        <v>1.2785193100000001</v>
+        <v>8.7256803789062509</v>
       </c>
       <c r="G33" s="10"/>
       <c r="H33" s="5">
         <f>F32*J31</f>
-        <v>1.2521</v>
+        <v>3.4196562500000001</v>
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="2"/>
@@ -1468,28 +1468,28 @@
       </c>
       <c r="F35" s="7">
         <f>B30*D30</f>
-        <v>14.442</v>
+        <v>41.794687499999995</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H35" s="14">
         <f>H21+H22*0.01</f>
-        <v>1.2332000000000001</v>
+        <v>3.3763437500000002</v>
       </c>
       <c r="I35" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J35" s="7">
         <f>(F35*H35+F37*H37)</f>
-        <v>18.830974400000002</v>
+        <v>143.66485692382813</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L35" s="14">
         <f>L21+L22*0.01</f>
-        <v>1.2521</v>
+        <v>3.4196562500000001</v>
       </c>
       <c r="M35" s="6" t="s">
         <v>11</v>
@@ -1506,24 +1506,24 @@
       <c r="E36" s="11"/>
       <c r="F36" s="1">
         <f>H35*J36</f>
-        <v>1.5440897200000001</v>
+        <v>11.545935006835938</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="5">
         <f>F35*J36</f>
-        <v>18.082828200000002</v>
+        <v>142.92346432617185</v>
       </c>
       <c r="I36" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J36" s="1">
         <f>L35*N31</f>
-        <v>1.2521</v>
+        <v>3.4196562500000001</v>
       </c>
       <c r="K36" s="12"/>
       <c r="L36" s="5">
         <f>J35*N31</f>
-        <v>18.830974400000002</v>
+        <v>143.66485692382813</v>
       </c>
       <c r="M36" s="11" t="s">
         <v>11</v>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="H37" s="14">
         <f>H23+H24*0.01</f>
-        <v>1.0211000000000001</v>
+        <v>2.551625</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>11</v>
@@ -1569,12 +1569,12 @@
       <c r="E38" s="9"/>
       <c r="F38" s="2">
         <f>H37*J36</f>
-        <v>1.2785193100000001</v>
+        <v>8.7256803789062509</v>
       </c>
       <c r="G38" s="10"/>
       <c r="H38" s="5">
         <f>F37*J36</f>
-        <v>1.2521</v>
+        <v>3.4196562500000001</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="2"/>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="L40" s="14">
         <f>L26+L27*0.01</f>
-        <v>1.02</v>
+        <v>2.5199999999999996</v>
       </c>
       <c r="M40" s="6" t="s">
         <v>11</v>
@@ -1634,7 +1634,7 @@
       <c r="I41" s="9"/>
       <c r="J41" s="2">
         <f>L40*N31</f>
-        <v>1.02</v>
+        <v>2.5199999999999996</v>
       </c>
       <c r="K41" s="10"/>
       <c r="L41" s="13">

</xml_diff>

<commit_message>
fixed Excel model, fixed tests
</commit_message>
<xml_diff>
--- a/model.xlsx
+++ b/model.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="14220" windowHeight="7815"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -79,7 +79,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,8 +110,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -223,11 +229,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -243,9 +288,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -258,9 +313,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -298,7 +353,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -370,7 +425,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -544,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +615,7 @@
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -583,54 +638,57 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="7">
-        <v>2.2000000000000002</v>
+        <v>10</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="5">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="7">
         <f>B2*D2</f>
-        <v>5.5</v>
+        <v>10</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="5">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="7">
         <f>(F2*H2+F4*H4)</f>
-        <v>16.25</v>
+        <v>11</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L2" s="5">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N2" s="8">
         <f>J2*L2+J7*L7+J12*L12</f>
-        <v>83.75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="O2" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
@@ -638,40 +696,45 @@
       <c r="C3" s="12"/>
       <c r="D3" s="5">
         <f>(F3+F8)*B2</f>
-        <v>27.500000000000004</v>
+        <v>-20</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="1">
         <f>H2*J3</f>
-        <v>6.25</v>
+        <v>-1</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="5">
         <f>J3*F2</f>
-        <v>13.75</v>
+        <v>-10</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J3" s="1">
         <f>L2*N3</f>
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="K3" s="12"/>
       <c r="L3" s="5">
         <f>J2*N3</f>
-        <v>16.25</v>
+        <v>-11</v>
       </c>
       <c r="M3" s="11" t="s">
         <v>11</v>
       </c>
       <c r="N3" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <f>(1 - EXP(-1*(N2-O2)^2))*O3</f>
+        <v>-1</v>
+      </c>
+      <c r="O3" s="24">
+        <f>IF(N2&gt;O2, -1, 1)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -688,7 +751,7 @@
         <v>9</v>
       </c>
       <c r="H4" s="5">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>11</v>
@@ -701,24 +764,24 @@
       </c>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="10"/>
-      <c r="D5" s="5"/>
+      <c r="D5" s="15"/>
       <c r="E5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="2">
         <f>H4*J3</f>
-        <v>6.25</v>
+        <v>-1</v>
       </c>
       <c r="G5" s="10"/>
-      <c r="H5" s="5">
+      <c r="H5" s="15">
         <f>F4*J3</f>
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="2"/>
@@ -729,97 +792,97 @@
       </c>
       <c r="N5" s="10"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D6" s="4"/>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D6" s="17"/>
       <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="4"/>
+      <c r="H6" s="17"/>
       <c r="L6" s="4"/>
       <c r="M6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6" t="s">
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="7">
         <f>B2*D2</f>
-        <v>5.5</v>
+        <v>10</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="5">
-        <v>2.5</v>
+      <c r="H7" s="3">
+        <v>1</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J7" s="7">
         <f>(F7*H7+F9*H9)</f>
-        <v>16.25</v>
+        <v>11</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L7" s="5">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N7" s="8"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="11"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="1">
         <f>H7*J8</f>
-        <v>6.25</v>
+        <v>-1</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="5">
         <f>F7*J8</f>
-        <v>13.75</v>
+        <v>-10</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J8" s="1">
         <f>L7*N3</f>
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="K8" s="12"/>
       <c r="L8" s="5">
         <f>J7*N3</f>
-        <v>16.25</v>
+        <v>-11</v>
       </c>
       <c r="M8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="N8" s="12"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="7">
         <v>1</v>
       </c>
@@ -827,7 +890,7 @@
         <v>9</v>
       </c>
       <c r="H9" s="5">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>11</v>
@@ -840,22 +903,22 @@
       </c>
       <c r="N9" s="8"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="9"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="2"/>
       <c r="F10" s="2">
         <f>H9*J8</f>
-        <v>6.25</v>
+        <v>-1</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="5">
         <f>F9*J8</f>
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="2"/>
@@ -866,26 +929,26 @@
       </c>
       <c r="N10" s="10"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D11" s="4"/>
-      <c r="H11" s="4"/>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D11" s="17"/>
+      <c r="H11" s="17"/>
       <c r="L11" s="4"/>
       <c r="M11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="7"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="7"/>
       <c r="J12" s="7">
         <v>1</v>
       </c>
@@ -893,38 +956,41 @@
         <v>9</v>
       </c>
       <c r="L12" s="5">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="M12" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N12" s="8"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="9"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="9"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="2"/>
       <c r="J13" s="2">
         <f>L12*N3</f>
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="13">
         <f>J12*N3</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="M13" s="9"/>
       <c r="N13" s="10"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D14" s="18"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D15" s="3" t="s">
         <v>1</v>
       </c>
@@ -935,11 +1001,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="7">
+        <f>B2</f>
         <v>10</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -947,45 +1014,49 @@
       </c>
       <c r="D16" s="14">
         <f>D2+D3*0.01</f>
-        <v>2.7749999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="7">
         <f>B16*D16</f>
-        <v>27.75</v>
+        <v>8</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="14">
         <f>H2+H3*0.01</f>
-        <v>2.6375000000000002</v>
+        <v>0.9</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J16" s="7">
         <f>(F16*H16+F18*H18)</f>
-        <v>75.715625000000017</v>
+        <v>8.19</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L16" s="14">
         <f>L2+L3*0.01</f>
-        <v>2.6625000000000001</v>
+        <v>0.89</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N16" s="8">
         <f>J16*L16+J21*L21+J26*L26</f>
-        <v>405.69570312500008</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>15.568199999999999</v>
+      </c>
+      <c r="O16" s="24">
+        <f>O2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>8</v>
       </c>
@@ -993,40 +1064,45 @@
       <c r="C17" s="12"/>
       <c r="D17" s="5">
         <f>(F17+F22)*B16</f>
-        <v>140.44687500000003</v>
+        <v>-16.02</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="1">
         <f>H16*J17</f>
-        <v>7.022343750000001</v>
+        <v>-0.80100000000000005</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="5">
         <f>J17*F16</f>
-        <v>73.884375000000006</v>
+        <v>-7.12</v>
       </c>
       <c r="I17" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J17" s="1">
         <f>L16*N17</f>
-        <v>2.6625000000000001</v>
+        <v>-0.89</v>
       </c>
       <c r="K17" s="12"/>
       <c r="L17" s="5">
         <f>J16*N17</f>
-        <v>75.715625000000017</v>
+        <v>-8.19</v>
       </c>
       <c r="M17" s="11" t="s">
         <v>11</v>
       </c>
       <c r="N17" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+        <f>(1 - EXP(-1*(N16-O16)^2))*O17</f>
+        <v>-1</v>
+      </c>
+      <c r="O17" s="24">
+        <f>IF(N16&gt;O16, -1, 1)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>7</v>
       </c>
@@ -1044,7 +1120,7 @@
       </c>
       <c r="H18" s="14">
         <f>H4+H5*0.01</f>
-        <v>2.5249999999999999</v>
+        <v>0.99</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>11</v>
@@ -1057,24 +1133,24 @@
       </c>
       <c r="N18" s="8"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="10"/>
-      <c r="D19" s="5"/>
+      <c r="D19" s="15"/>
       <c r="E19" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F19" s="2">
         <f>H18*J17</f>
-        <v>6.7228124999999999</v>
+        <v>-0.88109999999999999</v>
       </c>
       <c r="G19" s="10"/>
-      <c r="H19" s="5">
+      <c r="H19" s="15">
         <f>F18*J17</f>
-        <v>2.6625000000000001</v>
+        <v>-0.89</v>
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="2"/>
@@ -1085,99 +1161,99 @@
       </c>
       <c r="N19" s="10"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D20" s="4"/>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D20" s="17"/>
       <c r="E20" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="4"/>
+      <c r="H20" s="17"/>
       <c r="L20" s="4"/>
       <c r="M20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6" t="s">
+      <c r="C21" s="7"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="7">
         <f>B16*D16</f>
-        <v>27.75</v>
+        <v>8</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H21" s="16">
         <f>H7+H8*0.01</f>
-        <v>2.6375000000000002</v>
+        <v>0.9</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J21" s="7">
         <f>(F21*H21+F23*H23)</f>
-        <v>75.715625000000017</v>
+        <v>8.19</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L21" s="14">
         <f>L7+L8*0.01</f>
-        <v>2.6625000000000001</v>
+        <v>0.89</v>
       </c>
       <c r="M21" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N21" s="8"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="11"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="1"/>
       <c r="F22" s="1">
         <f>H21*J22</f>
-        <v>7.022343750000001</v>
+        <v>-0.80100000000000005</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="5">
         <f>F21*J22</f>
-        <v>73.884375000000006</v>
+        <v>-7.12</v>
       </c>
       <c r="I22" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J22" s="1">
         <f>L21*N17</f>
-        <v>2.6625000000000001</v>
+        <v>-0.89</v>
       </c>
       <c r="K22" s="12"/>
       <c r="L22" s="5">
         <f>J21*N17</f>
-        <v>75.715625000000017</v>
+        <v>-8.19</v>
       </c>
       <c r="M22" s="11" t="s">
         <v>11</v>
       </c>
       <c r="N22" s="12"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="7"/>
       <c r="F23" s="7">
         <v>1</v>
       </c>
@@ -1186,7 +1262,7 @@
       </c>
       <c r="H23" s="14">
         <f>H9+H10*0.01</f>
-        <v>2.5249999999999999</v>
+        <v>0.99</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>11</v>
@@ -1199,22 +1275,22 @@
       </c>
       <c r="N23" s="8"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="9"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="2"/>
       <c r="F24" s="2">
         <f>H23*J22</f>
-        <v>6.7228124999999999</v>
+        <v>-0.88109999999999999</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="5">
         <f>F23*J22</f>
-        <v>2.6625000000000001</v>
+        <v>-0.89</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="2"/>
@@ -1225,26 +1301,26 @@
       </c>
       <c r="N24" s="10"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D25" s="4"/>
-      <c r="H25" s="4"/>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D25" s="17"/>
+      <c r="H25" s="17"/>
       <c r="L25" s="4"/>
       <c r="M25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="7"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="6"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="7"/>
       <c r="J26" s="7">
         <v>1</v>
       </c>
@@ -1253,38 +1329,38 @@
       </c>
       <c r="L26" s="14">
         <f>L12+L13*0.01</f>
-        <v>2.5099999999999998</v>
+        <v>0.99</v>
       </c>
       <c r="M26" s="6" t="s">
         <v>11</v>
       </c>
       <c r="N26" s="8"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="9"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="2"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="9"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="2"/>
       <c r="J27" s="2">
         <f>L26*N17</f>
-        <v>2.5099999999999998</v>
+        <v>-0.99</v>
       </c>
       <c r="K27" s="10"/>
       <c r="L27" s="13">
         <f>J26*N17</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="M27" s="9"/>
       <c r="N27" s="10"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D29" s="3" t="s">
         <v>1</v>
       </c>
@@ -1295,11 +1371,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="7">
+        <f>B2</f>
         <v>10</v>
       </c>
       <c r="C30" s="8" t="s">
@@ -1307,45 +1384,49 @@
       </c>
       <c r="D30" s="14">
         <f>D16+D17*0.01</f>
-        <v>4.1794687499999998</v>
+        <v>0.63980000000000004</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F30" s="7">
         <f>B30*D30</f>
-        <v>41.794687499999995</v>
+        <v>6.3980000000000006</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H30" s="14">
         <f>H16+H17*0.01</f>
-        <v>3.3763437500000002</v>
+        <v>0.82879999999999998</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J30" s="7">
         <f>(F30*H30+F32*H32)</f>
-        <v>143.66485692382813</v>
+        <v>6.2837623999999996</v>
       </c>
       <c r="K30" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L30" s="14">
         <f>L16+L17*0.01</f>
-        <v>3.4196562500000001</v>
+        <v>0.80810000000000004</v>
       </c>
       <c r="M30" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N30" s="8">
         <f>J30*L30+J35*L35+J40*L40</f>
-        <v>985.08885176984927</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+        <v>11.13581679088</v>
+      </c>
+      <c r="O30" s="24">
+        <f>O2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>8</v>
       </c>
@@ -1353,40 +1434,45 @@
       <c r="C31" s="12"/>
       <c r="D31" s="5">
         <f>(F31+F36)*B30</f>
-        <v>230.91870013671877</v>
+        <v>-13.395065600000001</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F31" s="1">
         <f>H30*J31</f>
-        <v>11.545935006835938</v>
+        <v>-0.66975328000000001</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="5">
         <f>J31*F30</f>
-        <v>142.92346432617185</v>
+        <v>-5.1702238000000005</v>
       </c>
       <c r="I31" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J31" s="1">
         <f>L30*N31</f>
-        <v>3.4196562500000001</v>
+        <v>-0.80810000000000004</v>
       </c>
       <c r="K31" s="12"/>
       <c r="L31" s="5">
         <f>J30*N31</f>
-        <v>143.66485692382813</v>
+        <v>-6.2837623999999996</v>
       </c>
       <c r="M31" s="11" t="s">
         <v>11</v>
       </c>
       <c r="N31" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+        <f>(1 - EXP(-1*(N30-O30)^2))*O31</f>
+        <v>-1</v>
+      </c>
+      <c r="O31" s="24">
+        <f>IF(N30&gt;O30, -1, 1)</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>7</v>
       </c>
@@ -1404,7 +1490,7 @@
       </c>
       <c r="H32" s="14">
         <f>H18+H19*0.01</f>
-        <v>2.551625</v>
+        <v>0.98109999999999997</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>11</v>
@@ -1423,18 +1509,18 @@
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="10"/>
-      <c r="D33" s="5"/>
+      <c r="D33" s="15"/>
       <c r="E33" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F33" s="2">
         <f>H32*J31</f>
-        <v>8.7256803789062509</v>
+        <v>-0.79282691000000005</v>
       </c>
       <c r="G33" s="10"/>
-      <c r="H33" s="5">
+      <c r="H33" s="4">
         <f>F32*J31</f>
-        <v>3.4196562500000001</v>
+        <v>-0.80810000000000004</v>
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="2"/>
@@ -1446,11 +1532,11 @@
       <c r="N33" s="10"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D34" s="4"/>
+      <c r="D34" s="17"/>
       <c r="E34" t="s">
         <v>10</v>
       </c>
-      <c r="H34" s="4"/>
+      <c r="H34" s="23"/>
       <c r="L34" s="4"/>
       <c r="M34" t="s">
         <v>11</v>
@@ -1461,35 +1547,35 @@
         <v>7</v>
       </c>
       <c r="B35" s="7"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="6" t="s">
+      <c r="C35" s="7"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F35" s="7">
         <f>B30*D30</f>
-        <v>41.794687499999995</v>
+        <v>6.3980000000000006</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H35" s="14">
+      <c r="H35" s="22">
         <f>H21+H22*0.01</f>
-        <v>3.3763437500000002</v>
+        <v>0.82879999999999998</v>
       </c>
       <c r="I35" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J35" s="7">
         <f>(F35*H35+F37*H37)</f>
-        <v>143.66485692382813</v>
+        <v>6.2837623999999996</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L35" s="14">
         <f>L21+L22*0.01</f>
-        <v>3.4196562500000001</v>
+        <v>0.80810000000000004</v>
       </c>
       <c r="M35" s="6" t="s">
         <v>11</v>
@@ -1501,29 +1587,29 @@
         <v>8</v>
       </c>
       <c r="B36" s="1"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="11"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="1"/>
       <c r="F36" s="1">
         <f>H35*J36</f>
-        <v>11.545935006835938</v>
+        <v>-0.66975328000000001</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="5">
         <f>F35*J36</f>
-        <v>142.92346432617185</v>
+        <v>-5.1702238000000005</v>
       </c>
       <c r="I36" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J36" s="1">
         <f>L35*N31</f>
-        <v>3.4196562500000001</v>
+        <v>-0.80810000000000004</v>
       </c>
       <c r="K36" s="12"/>
       <c r="L36" s="5">
         <f>J35*N31</f>
-        <v>143.66485692382813</v>
+        <v>-6.2837623999999996</v>
       </c>
       <c r="M36" s="11" t="s">
         <v>11</v>
@@ -1535,9 +1621,9 @@
         <v>7</v>
       </c>
       <c r="B37" s="7"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="6"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="7"/>
       <c r="F37" s="7">
         <v>1</v>
       </c>
@@ -1546,7 +1632,7 @@
       </c>
       <c r="H37" s="14">
         <f>H23+H24*0.01</f>
-        <v>2.551625</v>
+        <v>0.98109999999999997</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>11</v>
@@ -1564,17 +1650,17 @@
         <v>8</v>
       </c>
       <c r="B38" s="2"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="9"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="2"/>
       <c r="F38" s="2">
         <f>H37*J36</f>
-        <v>8.7256803789062509</v>
+        <v>-0.79282691000000005</v>
       </c>
       <c r="G38" s="10"/>
       <c r="H38" s="5">
         <f>F37*J36</f>
-        <v>3.4196562500000001</v>
+        <v>-0.80810000000000004</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="2"/>
@@ -1586,7 +1672,7 @@
       <c r="N38" s="10"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D39" s="4"/>
+      <c r="D39" s="17"/>
       <c r="H39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" t="s">
@@ -1598,13 +1684,13 @@
         <v>7</v>
       </c>
       <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="7"/>
       <c r="F40" s="7"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="6"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="7"/>
       <c r="J40" s="7">
         <v>1</v>
       </c>
@@ -1613,7 +1699,7 @@
       </c>
       <c r="L40" s="14">
         <f>L26+L27*0.01</f>
-        <v>2.5199999999999996</v>
+        <v>0.98</v>
       </c>
       <c r="M40" s="6" t="s">
         <v>11</v>
@@ -1625,21 +1711,21 @@
         <v>8</v>
       </c>
       <c r="B41" s="2"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="9"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="2"/>
       <c r="F41" s="2"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="9"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="2"/>
       <c r="J41" s="2">
         <f>L40*N31</f>
-        <v>2.5199999999999996</v>
+        <v>-0.98</v>
       </c>
       <c r="K41" s="10"/>
       <c r="L41" s="13">
         <f>J40*N31</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="M41" s="9"/>
       <c r="N41" s="10"/>

</xml_diff>

<commit_message>
finished almost all tests, TODO:wrong-type-error tests
</commit_message>
<xml_diff>
--- a/model.xlsx
+++ b/model.xlsx
@@ -602,7 +602,7 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,49 +643,49 @@
         <v>7</v>
       </c>
       <c r="B2" s="7">
-        <v>10</v>
+        <v>5.6</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="5">
-        <v>1</v>
+        <v>-2.1</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="7">
-        <f>B2*D2</f>
-        <v>10</v>
+        <f>IF(B2*D2&gt;0,B2*D2,0.01*B2*D2)</f>
+        <v>-0.1176</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="5">
-        <v>1</v>
+        <v>-2.1</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="7">
-        <f>(F2*H2+F4*H4)</f>
-        <v>11</v>
+        <f>IF(F2*H2+F4*H4&gt;0,F2*H2+F4*H4,0.01*(F2*H2+F4*H4))</f>
+        <v>-1.8530399999999999E-2</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L2" s="5">
-        <v>1</v>
+        <v>-2.1</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N2" s="8">
-        <f>J2*L2+J7*L7+J12*L12</f>
-        <v>23</v>
+        <f>IF((J2*L2+J7*L7+J12*L12)&gt;0,(J2*L2+J7*L7+J12*L12),0.01*(J2*L2+J7*L7+J12*L12))</f>
+        <v>-2.0221723200000003E-2</v>
       </c>
       <c r="O2" s="24">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -695,43 +695,43 @@
       <c r="B3" s="1"/>
       <c r="C3" s="12"/>
       <c r="D3" s="5">
-        <f>(F3+F8)*B2</f>
-        <v>-20</v>
+        <f>IF(B2*D2&gt;0,((F3+F8)*B2),0.01*((F3+F8)*B2))</f>
+        <v>4.9392000000000004E-5</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="1">
-        <f>H2*J3</f>
-        <v>-1</v>
+        <f>IF(F2*H2+F4*H4&gt;0,H2*J3,0.01*(H2*J3))</f>
+        <v>4.4100000000000009E-4</v>
       </c>
       <c r="G3" s="12"/>
       <c r="H3" s="5">
-        <f>J3*F2</f>
-        <v>-10</v>
+        <f>IF(F2*H2+F4*H4&gt;0,(F2*J3),0.01*(F2*J3))</f>
+        <v>2.4696000000000002E-5</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J3" s="1">
-        <f>L2*N3</f>
-        <v>-1</v>
+        <f>IF((J2*L2+J7*L7+J12*L12)&gt;0,(L2*N3),0.01*(L2*N3))</f>
+        <v>-2.1000000000000001E-2</v>
       </c>
       <c r="K3" s="12"/>
       <c r="L3" s="5">
-        <f>J2*N3</f>
-        <v>-11</v>
+        <f>IF((J2*L2+J7*L7+J12*L12)&gt;0,(J2*N3),0.01*(J2*N3))</f>
+        <v>-1.8530399999999999E-4</v>
       </c>
       <c r="M3" s="11" t="s">
         <v>11</v>
       </c>
       <c r="N3" s="12">
         <f>(1 - EXP(-1*(N2-O2)^2))*O3</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="O3" s="24">
         <f>IF(N2&gt;O2, -1, 1)</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -751,7 +751,7 @@
         <v>9</v>
       </c>
       <c r="H4" s="5">
-        <v>1</v>
+        <v>-2.1</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>11</v>
@@ -775,13 +775,13 @@
         <v>10</v>
       </c>
       <c r="F5" s="2">
-        <f>H4*J3</f>
-        <v>-1</v>
+        <f>IF(F2*H2+F4*H4&gt;0,H4*J3,0.01*(H4*J3))</f>
+        <v>4.4100000000000009E-4</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="15">
-        <f>F4*J3</f>
-        <v>-1</v>
+        <f>IF(F2*H2+F4*H4&gt;0,(F4*J3),0.01*(F4*J3))</f>
+        <v>-2.1000000000000001E-4</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="2"/>
@@ -814,27 +814,27 @@
         <v>12</v>
       </c>
       <c r="F7" s="7">
-        <f>B2*D2</f>
-        <v>10</v>
+        <f>IF(B2*D2&gt;0,B2*D2,0.01*B2*D2)</f>
+        <v>-0.1176</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="3">
-        <v>1</v>
+      <c r="H7" s="5">
+        <v>-2.1</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J7" s="7">
-        <f>(F7*H7+F9*H9)</f>
-        <v>11</v>
+        <f>IF(F7*H7+F9*H9&gt;0,F7*H7+F9*H9,0.01*(F7*H7+F9*H9))</f>
+        <v>-1.8530399999999999E-2</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L7" s="5">
-        <v>1</v>
+        <v>-2.1</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>11</v>
@@ -850,25 +850,25 @@
       <c r="D8" s="21"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
-        <f>H7*J8</f>
-        <v>-1</v>
+        <f>IF(F7*H7+F9*H9&gt;0,H7*J8,0.01*(H7*J8))</f>
+        <v>4.4100000000000009E-4</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="5">
-        <f>F7*J8</f>
-        <v>-10</v>
+        <f>IF(F7*H7+F9*H9&gt;0,(F7*J8),0.01*(F7*J8))</f>
+        <v>2.4696000000000002E-5</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J8" s="1">
-        <f>L7*N3</f>
-        <v>-1</v>
+        <f>IF((J2*L2+J7*L7+J12*L12)&gt;0,L7*N3,0.01*L7*N3)</f>
+        <v>-2.1000000000000001E-2</v>
       </c>
       <c r="K8" s="12"/>
       <c r="L8" s="5">
-        <f>J7*N3</f>
-        <v>-11</v>
+        <f>IF((J2*L2+J7*L7+J12*L12)&gt;0,(J7*N3),0.01*(J7*N3))</f>
+        <v>-1.8530399999999999E-4</v>
       </c>
       <c r="M8" s="11" t="s">
         <v>11</v>
@@ -890,7 +890,7 @@
         <v>9</v>
       </c>
       <c r="H9" s="5">
-        <v>1</v>
+        <v>-2.1</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>11</v>
@@ -912,13 +912,13 @@
       <c r="D10" s="21"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2">
-        <f>H9*J8</f>
-        <v>-1</v>
+        <f>IF(F7*H7+F9*H9&gt;0,H9*J8,0.01*(H9*J8))</f>
+        <v>4.4100000000000009E-4</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="5">
-        <f>F9*J8</f>
-        <v>-1</v>
+        <f>IF(F7*H7+F9*H9&gt;0,(F9*J8),(F9*J8)*0.01)</f>
+        <v>-2.1000000000000001E-4</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="2"/>
@@ -956,7 +956,7 @@
         <v>9</v>
       </c>
       <c r="L12" s="5">
-        <v>1</v>
+        <v>-2.1</v>
       </c>
       <c r="M12" s="6" t="s">
         <v>11</v>
@@ -976,13 +976,13 @@
       <c r="H13" s="21"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2">
-        <f>L12*N3</f>
-        <v>-1</v>
+        <f>IF((J2*L2+J7*L7+J12*L12)&gt;0,L12*N3,0.01*(L12*N3))</f>
+        <v>-2.1000000000000001E-2</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="13">
-        <f>J12*N3</f>
-        <v>-1</v>
+        <f>IF((J2*L2+J7*L7+J12*L12)&gt;0,(J12*N3),0.01*(J12*N3))</f>
+        <v>0.01</v>
       </c>
       <c r="M13" s="9"/>
       <c r="N13" s="10"/>
@@ -1007,53 +1007,53 @@
       </c>
       <c r="B16" s="7">
         <f>B2</f>
-        <v>10</v>
+        <v>5.6</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="14">
         <f>D2+D3*0.01</f>
-        <v>0.8</v>
+        <v>-2.0999995060800001</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="7">
-        <f>B16*D16</f>
-        <v>8</v>
+        <f>IF(B16*D16&gt;0,B16*D16,0.01*B16*D16)</f>
+        <v>-0.11759997234047999</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="14">
         <f>H2+H3*0.01</f>
-        <v>0.9</v>
+        <v>-2.0999997530400001</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J16" s="7">
-        <f>(F16*H16+F18*H18)</f>
-        <v>8.19</v>
+        <f>IF(F16*H16+F18*H18&gt;0,F16*H16+F18*H18,0.01*(F16*H16+F18*H18))</f>
+        <v>-1.8530421871274814E-2</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L16" s="14">
         <f>L2+L3*0.01</f>
-        <v>0.89</v>
+        <v>-2.1000018530400002</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N16" s="8">
-        <f>J16*L16+J21*L21+J26*L26</f>
-        <v>15.568199999999999</v>
+        <f>IF((J16*L16+J21*L21+J26*L26)&gt;0,(J16*L16+J21*L21+J26*L26),0.01*(J16*L16+J21*L21+J26*L26))</f>
+        <v>-2.0220721594654198E-2</v>
       </c>
       <c r="O16" s="24">
         <f>O2</f>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1064,42 +1064,42 @@
       <c r="C17" s="12"/>
       <c r="D17" s="5">
         <f>(F17+F22)*B16</f>
-        <v>-16.02</v>
+        <v>49.392037774996474</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="1">
         <f>H16*J17</f>
-        <v>-0.80100000000000005</v>
+        <v>4.4100033727675427</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="5">
         <f>J17*F16</f>
-        <v>-7.12</v>
+        <v>0.24696015983246075</v>
       </c>
       <c r="I17" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J17" s="1">
         <f>L16*N17</f>
-        <v>-0.89</v>
+        <v>-2.1000018530400002</v>
       </c>
       <c r="K17" s="12"/>
       <c r="L17" s="5">
         <f>J16*N17</f>
-        <v>-8.19</v>
+        <v>-1.8530421871274814E-2</v>
       </c>
       <c r="M17" s="11" t="s">
         <v>11</v>
       </c>
       <c r="N17" s="12">
         <f>(1 - EXP(-1*(N16-O16)^2))*O17</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="O17" s="24">
         <f>IF(N16&gt;O16, -1, 1)</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -1120,7 +1120,7 @@
       </c>
       <c r="H18" s="14">
         <f>H4+H5*0.01</f>
-        <v>0.99</v>
+        <v>-2.1000021000000002</v>
       </c>
       <c r="I18" s="6" t="s">
         <v>11</v>
@@ -1145,12 +1145,12 @@
       </c>
       <c r="F19" s="2">
         <f>H18*J17</f>
-        <v>-0.88109999999999999</v>
+        <v>4.4100083013878919</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="15">
         <f>F18*J17</f>
-        <v>-0.89</v>
+        <v>-2.1000018530400002</v>
       </c>
       <c r="I19" s="9"/>
       <c r="J19" s="2"/>
@@ -1183,29 +1183,29 @@
         <v>12</v>
       </c>
       <c r="F21" s="7">
-        <f>B16*D16</f>
-        <v>8</v>
+        <f>IF(B16*D16&gt;0,B16*D16,0.01*B16*D16)</f>
+        <v>-0.11759997234047999</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H21" s="16">
         <f>H7+H8*0.01</f>
-        <v>0.9</v>
+        <v>-2.0999997530400001</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J21" s="7">
-        <f>(F21*H21+F23*H23)</f>
-        <v>8.19</v>
+        <f>IF(F21*H21+F23*H23&gt;0,F21*H21+F23*H23,0.01*(F21*H21+F23*H23))</f>
+        <v>-1.8530421871274814E-2</v>
       </c>
       <c r="K21" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L21" s="14">
         <f>L7+L8*0.01</f>
-        <v>0.89</v>
+        <v>-2.1000018530400002</v>
       </c>
       <c r="M21" s="6" t="s">
         <v>11</v>
@@ -1222,24 +1222,24 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1">
         <f>H21*J22</f>
-        <v>-0.80100000000000005</v>
+        <v>4.4100033727675427</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="5">
         <f>F21*J22</f>
-        <v>-7.12</v>
+        <v>0.24696015983246075</v>
       </c>
       <c r="I22" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J22" s="1">
         <f>L21*N17</f>
-        <v>-0.89</v>
+        <v>-2.1000018530400002</v>
       </c>
       <c r="K22" s="12"/>
       <c r="L22" s="5">
         <f>J21*N17</f>
-        <v>-8.19</v>
+        <v>-1.8530421871274814E-2</v>
       </c>
       <c r="M22" s="11" t="s">
         <v>11</v>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="H23" s="14">
         <f>H9+H10*0.01</f>
-        <v>0.99</v>
+        <v>-2.1000021000000002</v>
       </c>
       <c r="I23" s="6" t="s">
         <v>11</v>
@@ -1285,12 +1285,12 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2">
         <f>H23*J22</f>
-        <v>-0.88109999999999999</v>
+        <v>4.4100083013878919</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="5">
         <f>F23*J22</f>
-        <v>-0.89</v>
+        <v>-2.1000018530400002</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="2"/>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="L26" s="14">
         <f>L12+L13*0.01</f>
-        <v>0.99</v>
+        <v>-2.0998999999999999</v>
       </c>
       <c r="M26" s="6" t="s">
         <v>11</v>
@@ -1350,12 +1350,12 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2">
         <f>L26*N17</f>
-        <v>-0.99</v>
+        <v>-2.0998999999999999</v>
       </c>
       <c r="K27" s="10"/>
       <c r="L27" s="13">
         <f>J26*N17</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="M27" s="9"/>
       <c r="N27" s="10"/>
@@ -1377,53 +1377,53 @@
       </c>
       <c r="B30" s="7">
         <f>B2</f>
-        <v>10</v>
+        <v>5.6</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="14">
         <f>D16+D17*0.01</f>
-        <v>0.63980000000000004</v>
+        <v>-1.6060791283300353</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F30" s="7">
-        <f>B30*D30</f>
-        <v>6.3980000000000006</v>
+        <f>IF(B30*D30&gt;0,B30*D30,0.01*B30*D30)</f>
+        <v>-8.994043118648197E-2</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H30" s="14">
         <f>H16+H17*0.01</f>
-        <v>0.82879999999999998</v>
+        <v>-2.0975301514416755</v>
       </c>
       <c r="I30" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J30" s="7">
-        <f>(F30*H30+F32*H32)</f>
-        <v>6.2837623999999996</v>
+        <f>IF(F30*H30+F32*H32&gt;0,F30*H30+F32*H32,0.01*(F30*H30+F32*H32))</f>
+        <v>-1.9323493522830887E-2</v>
       </c>
       <c r="K30" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L30" s="14">
         <f>L16+L17*0.01</f>
-        <v>0.80810000000000004</v>
+        <v>-2.1001871572587127</v>
       </c>
       <c r="M30" s="6" t="s">
         <v>12</v>
       </c>
       <c r="N30" s="8">
-        <f>J30*L30+J35*L35+J40*L40</f>
-        <v>11.13581679088</v>
+        <f>IF((J30*L30+J35*L35+J40*L40)&gt;0,(J30*L30+J35*L35+J40*L40),0.01*(J30*L30+J35*L35+J40*L40))</f>
+        <v>-2.0087340941399572E-2</v>
       </c>
       <c r="O30" s="24">
         <f>O2</f>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -1434,42 +1434,42 @@
       <c r="C31" s="12"/>
       <c r="D31" s="5">
         <f>(F31+F36)*B30</f>
-        <v>-13.395065600000001</v>
+        <v>49.338305923432173</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F31" s="1">
         <f>H30*J31</f>
-        <v>-0.66975328000000001</v>
+        <v>4.4052058860207302</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="5">
         <f>J31*F30</f>
-        <v>-5.1702238000000005</v>
+        <v>0.18889173849616045</v>
       </c>
       <c r="I31" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J31" s="1">
         <f>L30*N31</f>
-        <v>-0.80810000000000004</v>
+        <v>-2.1001871572587127</v>
       </c>
       <c r="K31" s="12"/>
       <c r="L31" s="5">
         <f>J30*N31</f>
-        <v>-6.2837623999999996</v>
+        <v>-1.9323493522830887E-2</v>
       </c>
       <c r="M31" s="11" t="s">
         <v>11</v>
       </c>
       <c r="N31" s="12">
         <f>(1 - EXP(-1*(N30-O30)^2))*O31</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="O31" s="24">
         <f>IF(N30&gt;O30, -1, 1)</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -1490,7 +1490,7 @@
       </c>
       <c r="H32" s="14">
         <f>H18+H19*0.01</f>
-        <v>0.98109999999999997</v>
+        <v>-2.1210021185304</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>11</v>
@@ -1515,12 +1515,12 @@
       </c>
       <c r="F33" s="2">
         <f>H32*J31</f>
-        <v>-0.79282691000000005</v>
+        <v>4.4545014098560678</v>
       </c>
       <c r="G33" s="10"/>
       <c r="H33" s="4">
         <f>F32*J31</f>
-        <v>-0.80810000000000004</v>
+        <v>-2.1001871572587127</v>
       </c>
       <c r="I33" s="9"/>
       <c r="J33" s="2"/>
@@ -1553,29 +1553,29 @@
         <v>12</v>
       </c>
       <c r="F35" s="7">
-        <f>B30*D30</f>
-        <v>6.3980000000000006</v>
+        <f>IF(B30*D30&gt;0,B30*D30,0.01*B30*D30)</f>
+        <v>-8.994043118648197E-2</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H35" s="22">
         <f>H21+H22*0.01</f>
-        <v>0.82879999999999998</v>
+        <v>-2.0975301514416755</v>
       </c>
       <c r="I35" s="6" t="s">
         <v>12</v>
       </c>
       <c r="J35" s="7">
-        <f>(F35*H35+F37*H37)</f>
-        <v>6.2837623999999996</v>
+        <f>IF(F35*H35+F37*H37&gt;0,F35*H35+F37*H37,0.01*(F35*H35+F37*H37))</f>
+        <v>-1.9323493522830887E-2</v>
       </c>
       <c r="K35" s="8" t="s">
         <v>9</v>
       </c>
       <c r="L35" s="14">
         <f>L21+L22*0.01</f>
-        <v>0.80810000000000004</v>
+        <v>-2.1001871572587127</v>
       </c>
       <c r="M35" s="6" t="s">
         <v>11</v>
@@ -1592,24 +1592,24 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1">
         <f>H35*J36</f>
-        <v>-0.66975328000000001</v>
+        <v>4.4052058860207302</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="5">
         <f>F35*J36</f>
-        <v>-5.1702238000000005</v>
+        <v>0.18889173849616045</v>
       </c>
       <c r="I36" s="11" t="s">
         <v>11</v>
       </c>
       <c r="J36" s="1">
         <f>L35*N31</f>
-        <v>-0.80810000000000004</v>
+        <v>-2.1001871572587127</v>
       </c>
       <c r="K36" s="12"/>
       <c r="L36" s="5">
         <f>J35*N31</f>
-        <v>-6.2837623999999996</v>
+        <v>-1.9323493522830887E-2</v>
       </c>
       <c r="M36" s="11" t="s">
         <v>11</v>
@@ -1632,7 +1632,7 @@
       </c>
       <c r="H37" s="14">
         <f>H23+H24*0.01</f>
-        <v>0.98109999999999997</v>
+        <v>-2.1210021185304</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>11</v>
@@ -1655,12 +1655,12 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2">
         <f>H37*J36</f>
-        <v>-0.79282691000000005</v>
+        <v>4.4545014098560678</v>
       </c>
       <c r="G38" s="10"/>
       <c r="H38" s="5">
         <f>F37*J36</f>
-        <v>-0.80810000000000004</v>
+        <v>-2.1001871572587127</v>
       </c>
       <c r="I38" s="9"/>
       <c r="J38" s="2"/>
@@ -1699,7 +1699,7 @@
       </c>
       <c r="L40" s="14">
         <f>L26+L27*0.01</f>
-        <v>0.98</v>
+        <v>-2.0899000000000001</v>
       </c>
       <c r="M40" s="6" t="s">
         <v>11</v>
@@ -1720,12 +1720,12 @@
       <c r="I41" s="2"/>
       <c r="J41" s="2">
         <f>L40*N31</f>
-        <v>-0.98</v>
+        <v>-2.0899000000000001</v>
       </c>
       <c r="K41" s="10"/>
       <c r="L41" s="13">
         <f>J40*N31</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="M41" s="9"/>
       <c r="N41" s="10"/>

</xml_diff>